<commit_message>
Chunked graph performance improvements.
</commit_message>
<xml_diff>
--- a/RunTimes.xlsx
+++ b/RunTimes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Egyetem\Projektmunka\LTown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D56FA3-90B9-4A17-9130-E6C7626A3287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C59A6A-76AC-48E5-9047-53D4EE42EBD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4965" yWindow="1245" windowWidth="15795" windowHeight="13590" xr2:uid="{3C8EEE7A-615B-4858-911D-5130FDF9A387}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>Run times</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>Map datatype(Version 3)</t>
+  </si>
+  <si>
+    <t>Map datatype(Version 4)</t>
+  </si>
+  <si>
+    <t>Map datatype(Version 5)</t>
   </si>
 </sst>
 </file>
@@ -106,10 +112,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36213C59-6030-4E53-BC54-010B961CD5F2}">
-  <dimension ref="A2:F11"/>
+  <dimension ref="A2:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,10 +445,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -465,10 +471,10 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>3.0555555555555555E-2</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>1.3888888888888889E-3</v>
       </c>
       <c r="D4" t="s">
@@ -485,10 +491,10 @@
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>9.4444444444444442E-2</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>7.2916666666666671E-2</v>
       </c>
       <c r="D5" t="s">
@@ -505,10 +511,10 @@
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>1.1111111111111112E-2</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>1.5972222222222224E-2</v>
       </c>
       <c r="D6" t="s">
@@ -525,10 +531,10 @@
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>8.6805555555555566E-2</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>6.8749999999999992E-2</v>
       </c>
       <c r="D7" t="s">
@@ -545,10 +551,10 @@
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>0.63888888888888895</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>1.1805555555555555E-2</v>
       </c>
       <c r="D8" t="s">
@@ -565,10 +571,10 @@
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>1.3194444444444444E-2</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>6.9444444444444447E-4</v>
       </c>
       <c r="D9" t="s">
@@ -585,10 +591,10 @@
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>0</v>
       </c>
       <c r="D10" t="s">
@@ -605,10 +611,10 @@
       <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>9.0972222222222218E-2</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>0</v>
       </c>
       <c r="D11" t="s">
@@ -618,6 +624,106 @@
         <v>20</v>
       </c>
       <c r="F11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1">
+        <v>6.2499999999999995E-3</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1">
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1">
+        <v>4.9305555555555554E-2</v>
+      </c>
+      <c r="C14" s="1">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14">
+        <v>20</v>
+      </c>
+      <c r="F14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1">
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15">
+        <v>20</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16">
+        <v>20</v>
+      </c>
+      <c r="F16">
         <v>7</v>
       </c>
     </row>

</xml_diff>